<commit_message>
Implement dynamic debounce logic in Airflow DAG with file watcher fallback
</commit_message>
<xml_diff>
--- a/data/incoming/BigData.xlsx
+++ b/data/incoming/BigData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharvilarjunwadkar/Downloads/Projects/legacy_to_modern_pipeline/data/incoming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC3B66-4806-A747-891B-B13253337F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC2AD4-3B6A-8D48-8A54-6E18042F7905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16120" xr2:uid="{908BC8D2-2B3E-0841-9221-DD45720E682F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{908BC8D2-2B3E-0841-9221-DD45720E682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Dummy_BigData_xlsx_Preview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>District</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>TX2025-002</t>
+  </si>
+  <si>
+    <t>1234-56-791</t>
+  </si>
+  <si>
+    <t>PID003</t>
+  </si>
+  <si>
+    <t>I-37</t>
+  </si>
+  <si>
+    <t>Cat 4</t>
+  </si>
+  <si>
+    <t>TX2025-003</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A492923-F4D7-5647-ADEC-480F59819A2E}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,6 +1526,98 @@
         <v>1150001</v>
       </c>
     </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>2027</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45933</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6">
+        <v>1200002.5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6">
+        <v>1100002</v>
+      </c>
+      <c r="S6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" t="s">
+        <v>56</v>
+      </c>
+      <c r="U6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6">
+        <v>300000</v>
+      </c>
+      <c r="X6">
+        <v>250000</v>
+      </c>
+      <c r="Y6">
+        <v>100000</v>
+      </c>
+      <c r="Z6">
+        <v>200000</v>
+      </c>
+      <c r="AA6">
+        <v>50000</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>45994</v>
+      </c>
+      <c r="AD6">
+        <v>1150002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>